<commit_message>
added rotating empty button
</commit_message>
<xml_diff>
--- a/assets/texts/texts.xlsx
+++ b/assets/texts/texts.xlsx
@@ -1,136 +1,179 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANP\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr autoCompressPictures="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Typography" sheetId="1" r:id="rId1"/>
     <sheet name="Translation" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" fullPrecision="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="145621" calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" fullPrecision="0" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
-  <si>
-    <t>Font</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Bpp</t>
-  </si>
-  <si>
-    <t>TouchGFX - Typography Sheet</t>
-  </si>
-  <si>
-    <t>TouchGFX - Translation Sheet</t>
-  </si>
-  <si>
-    <t>Typography Name</t>
-  </si>
-  <si>
-    <t>Wildcard Ranges</t>
-  </si>
-  <si>
-    <t>Fallback Character</t>
-  </si>
-  <si>
-    <t>Wildcard Characters</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Example 1</t>
-  </si>
-  <si>
-    <t>Example 2</t>
-  </si>
-  <si>
-    <t>Example 3</t>
-  </si>
-  <si>
-    <t>The pixel size of the font as an integer</t>
-  </si>
-  <si>
-    <t>The bit depth of the font. Valid values are 1, 2, 4 and 8</t>
-  </si>
-  <si>
-    <t>The character to write if a glyph is missing at runtime (blank causes assert if glyph is missing)</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>skip</t>
-  </si>
-  <si>
-    <t>0x1234</t>
-  </si>
-  <si>
-    <t>The characters that are used in wildcard strings</t>
-  </si>
-  <si>
-    <t>1234567890.-</t>
-  </si>
-  <si>
-    <t>AMPM</t>
-  </si>
-  <si>
-    <t>Similar to "Wildcard Characters", but can be used to easily specify a range of characters</t>
-  </si>
-  <si>
-    <t>0-9,A-F</t>
-  </si>
-  <si>
-    <t>48-57,65-70</t>
-  </si>
-  <si>
-    <t>0x30-0x39,0x41-0x48</t>
-  </si>
-  <si>
-    <t>For more information read about "Using texts and fonts" on http://support.touchgfx.com/</t>
-  </si>
-  <si>
-    <t>Ellipsis Character</t>
-  </si>
-  <si>
-    <t>The character to insert when truncating long lines. See TextArea::setWideTextAction()</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>0x22EF</t>
-  </si>
-  <si>
-    <t>TEXT ID</t>
-  </si>
-  <si>
-    <t>TYPOGRAPHY NAME</t>
-  </si>
-  <si>
-    <t>ALIGNMENT</t>
-  </si>
-  <si>
-    <t>DIRECTION</t>
-  </si>
-  <si>
-    <t>GB</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="53">
+  <si>
+    <t xml:space="preserve">Font</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bpp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TouchGFX - Typography Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TouchGFX - Translation Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wildcard Ranges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fallback Character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wildcard Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pixel size of the font as an integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bit depth of the font. Valid values are 1, 2, 4 and 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The character to write if a glyph is missing at runtime (blank causes assert if glyph is missing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The characters that are used in wildcard strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234567890.-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar to "Wildcard Characters", but can be used to easily specify a range of characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48-57,65-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x30-0x39,0x41-0x48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For more information read about "Using texts and fonts" on http://support.touchgfx.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ellipsis Character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The character to insert when truncating long lines. See TextArea::setWideTextAction()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x22EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEXT ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYPOGRAPHY NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIRECTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verdana.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hej W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hej Erik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCB_____.TTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STENCIL.TTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seguisym.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HEJ ERIK</t>
   </si>
 </sst>
 </file>
@@ -1270,39 +1313,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0.28515625" customWidth="1"/>
+    <col min="1" max="1" width="0.28515625" style="0" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="84.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" style="0" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" style="0" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="0" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="0" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" style="0" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="0" customWidth="1"/>
+    <col min="12" max="12" width="84.7109375" style="0" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="0" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="0" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" style="0" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="129" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="129" hidden="1" customHeight="1">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1"/>
     </row>
-    <row r="2" spans="2:15" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="39.95" customHeight="1" thickBot="1">
       <c r="B2" s="24" t="s">
         <v>3</v>
       </c>
@@ -1314,7 +1357,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15.75" thickBot="1">
       <c r="B3" s="17" t="s">
         <v>5</v>
       </c>
@@ -1340,11 +1383,25 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
+    <row r="4" spans="2:15">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
       <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1361,11 +1418,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
+    <row r="5" spans="2:15">
       <c r="K5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1380,11 +1433,7 @@
       </c>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
+    <row r="6" spans="2:15">
       <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1399,7 +1448,7 @@
       </c>
       <c r="O6" s="10"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="K7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1416,7 +1465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1431,7 +1480,7 @@
       </c>
       <c r="O8" s="10"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="K9" s="11" t="s">
         <v>6</v>
       </c>
@@ -1448,7 +1497,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="K10" s="11" t="s">
         <v>28</v>
       </c>
@@ -1463,20 +1512,20 @@
       </c>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="L12" s="16" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
+  <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <tableParts count="2">
@@ -1487,25 +1536,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="0.42578125" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="0.42578125" style="0" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="0" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" style="0" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="0" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="0" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="0" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="3.75" customHeight="1"/>
+    <row r="2" spans="2:6" ht="33" customHeight="1">
       <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
@@ -1513,23 +1562,41 @@
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="2:6" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
+    <row r="3" spans="2:6" s="22" customFormat="1">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>